<commit_message>
Added second ATO fuse to PCB
- ughhhhhhhh
- Having a second ATO fuse socket on the PCB is necessary to drive the PCB at its full ampacity of 76A continuous, 80A instantaneous
</commit_message>
<xml_diff>
--- a/BatteryMonitor/PCB Design/BOM.xlsx
+++ b/BatteryMonitor/PCB Design/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\russe\Repositories\MIL\ReptileRover\BatteryMonitor\PCB Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841B24E8-2317-448D-A1C8-3C6010CB73A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED29402-EE33-48A4-98B5-64ED46C1D573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{5990C43E-B455-444D-86C0-B82E11A430FF}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>F1</t>
   </si>
   <si>
-    <t>F2</t>
-  </si>
-  <si>
     <t>J1, J2, J3</t>
   </si>
   <si>
@@ -640,6 +637,9 @@
   <si>
     <t>Estimated Parts Total (before fees):</t>
   </si>
+  <si>
+    <t>F2, F3</t>
+  </si>
 </sst>
 </file>
 
@@ -647,7 +647,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -724,7 +724,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -739,7 +739,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -747,14 +746,14 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1123,8 +1122,8 @@
   </sheetPr>
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" zeroHeight="1" x14ac:dyDescent="0.35"/>
@@ -1135,8 +1134,8 @@
     <col min="4" max="4" width="21.54296875" customWidth="1"/>
     <col min="5" max="5" width="2.6328125" customWidth="1"/>
     <col min="6" max="6" width="5.81640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="11.54296875" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="7" customWidth="1"/>
     <col min="9" max="9" width="2.6328125" customWidth="1"/>
     <col min="10" max="10" width="13.81640625" customWidth="1"/>
     <col min="12" max="13" width="12.26953125" customWidth="1"/>
@@ -1147,325 +1146,325 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="9">
+      <c r="B1" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" s="8">
         <f>SUM(H4:H62)</f>
-        <v>82.856999999999999</v>
+        <v>87.22699999999999</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
-      <c r="M1" s="6" t="s">
-        <v>190</v>
+      <c r="M1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B2" s="11" t="s">
-        <v>172</v>
+      <c r="B2" s="10" t="s">
+        <v>171</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="4">
         <v>3</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>0.42</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <f>G4*F4</f>
         <v>1.26</v>
       </c>
       <c r="J4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L4" t="s">
-        <v>170</v>
-      </c>
-      <c r="M4" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M4" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>0.67</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H60" si="0">G5*F5</f>
         <v>0.67</v>
       </c>
       <c r="J5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L5" t="s">
-        <v>170</v>
-      </c>
-      <c r="M5" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M5" s="6" t="b">
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F6" s="4">
         <v>13</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>0.11899999999999999</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>1.5469999999999999</v>
       </c>
       <c r="J6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L6" t="s">
-        <v>170</v>
-      </c>
-      <c r="M6" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M6" s="6" t="b">
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J7" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" t="s">
+        <v>169</v>
+      </c>
+      <c r="M7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
         <v>95</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="H7" s="8">
-        <f t="shared" si="0"/>
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="J7" t="s">
-        <v>132</v>
-      </c>
-      <c r="L7" t="s">
-        <v>170</v>
-      </c>
-      <c r="M7" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
         <v>68</v>
       </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>69</v>
-      </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="7">
         <v>0.36</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
       <c r="J8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L8" t="s">
-        <v>170</v>
-      </c>
-      <c r="M8" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M8" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9" s="4">
         <v>2</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>0.16</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
       <c r="J9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L9" t="s">
-        <v>170</v>
-      </c>
-      <c r="M9" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M9" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D10" t="s">
-        <v>67</v>
-      </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>0.38</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
       <c r="J10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L10" t="s">
-        <v>170</v>
-      </c>
-      <c r="M10" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M10" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" t="s">
         <v>107</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>108</v>
       </c>
-      <c r="D11" t="s">
-        <v>109</v>
-      </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>0.47</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <f t="shared" si="0"/>
         <v>0.47</v>
       </c>
       <c r="J11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L11" t="s">
-        <v>170</v>
-      </c>
-      <c r="M11" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M11" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -1473,328 +1472,328 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>0.36</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>0.36</v>
       </c>
       <c r="J12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L12" t="s">
-        <v>170</v>
-      </c>
-      <c r="M12" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M12" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="7">
         <v>1.54</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <f t="shared" si="0"/>
         <v>1.54</v>
       </c>
       <c r="J14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L14" t="s">
-        <v>170</v>
-      </c>
-      <c r="M14" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M14" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" t="s">
         <v>85</v>
-      </c>
-      <c r="C15" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" t="s">
-        <v>86</v>
       </c>
       <c r="F15" s="4">
         <v>2</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>0.12</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
       <c r="J15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L15" t="s">
-        <v>170</v>
-      </c>
-      <c r="M15" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M15" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F16" s="4">
         <v>4</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>0.1</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="J16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L16" t="s">
-        <v>170</v>
-      </c>
-      <c r="M16" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M16" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="4">
         <v>3</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="7">
         <v>0.1</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="7">
         <f t="shared" si="0"/>
         <v>0.30000000000000004</v>
       </c>
       <c r="J17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L17" t="s">
-        <v>170</v>
-      </c>
-      <c r="M17" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M17" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="7">
         <v>0.47</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="7">
         <f t="shared" si="0"/>
         <v>0.47</v>
       </c>
       <c r="J18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L18" t="s">
-        <v>170</v>
-      </c>
-      <c r="M18" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M18" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F19" s="4">
         <v>7</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="7">
         <v>0.1</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="7">
         <f t="shared" si="0"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="J19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L19" t="s">
-        <v>170</v>
-      </c>
-      <c r="M19" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M19" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="4">
         <v>2</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="7">
         <v>0.11</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
       <c r="J20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L20" t="s">
-        <v>170</v>
-      </c>
-      <c r="M20" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M20" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <v>0.1</v>
       </c>
-      <c r="H22" s="8">
+      <c r="H22" s="7">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="J22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L22" t="s">
-        <v>170</v>
-      </c>
-      <c r="M22" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M22" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
         <v>73</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>74</v>
       </c>
-      <c r="D23" t="s">
-        <v>75</v>
-      </c>
       <c r="F23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="7">
         <v>0.16</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="7">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
       <c r="J23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L23" t="s">
-        <v>170</v>
-      </c>
-      <c r="M23" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M23" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" t="s">
         <v>115</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>116</v>
       </c>
-      <c r="D24" t="s">
-        <v>117</v>
-      </c>
       <c r="F24" s="4">
         <v>1</v>
       </c>
-      <c r="G24" s="8">
+      <c r="G24" s="7">
         <v>0.93</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="7">
         <f t="shared" si="0"/>
         <v>0.93</v>
       </c>
       <c r="J24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L24" t="s">
-        <v>170</v>
-      </c>
-      <c r="M24" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M24" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1803,28 +1802,28 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F25" s="4">
         <v>2</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G25" s="7">
         <v>0.41</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="7">
         <f t="shared" si="0"/>
         <v>0.82</v>
       </c>
       <c r="J25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L25" t="s">
-        <v>170</v>
-      </c>
-      <c r="M25" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M25" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1837,7 +1836,7 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
@@ -1845,29 +1844,29 @@
       <c r="F27" s="4">
         <v>2</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="7">
         <v>0.12</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="7">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
       <c r="J27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L27" t="s">
-        <v>170</v>
-      </c>
-      <c r="M27" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M27" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
         <v>105</v>
-      </c>
-      <c r="C28" t="s">
-        <v>106</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
@@ -1875,29 +1874,29 @@
       <c r="F28" s="4">
         <v>1</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G28" s="7">
         <v>0.1</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="7">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
       <c r="J28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L28" t="s">
-        <v>170</v>
-      </c>
-      <c r="M28" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M28" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" t="s">
         <v>113</v>
-      </c>
-      <c r="C29" t="s">
-        <v>114</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
@@ -1905,106 +1904,106 @@
       <c r="F29" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="7">
         <v>0.32</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="7">
         <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
       <c r="J29" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L29" t="s">
-        <v>170</v>
-      </c>
-      <c r="M29" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M29" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F31" s="4">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L31" t="s">
-        <v>171</v>
-      </c>
-      <c r="M31" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M31" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" t="s">
         <v>56</v>
       </c>
-      <c r="C32" t="s">
-        <v>143</v>
-      </c>
-      <c r="D32" t="s">
-        <v>57</v>
-      </c>
       <c r="F32" s="4">
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L32" t="s">
-        <v>171</v>
-      </c>
-      <c r="M32" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M32" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F33" s="4">
         <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L33" t="s">
-        <v>171</v>
-      </c>
-      <c r="M33" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M33" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35"/>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D35" t="s">
         <v>23</v>
@@ -2012,20 +2011,20 @@
       <c r="F35" s="4">
         <v>1</v>
       </c>
-      <c r="G35" s="8">
+      <c r="G35" s="7">
         <v>0.19</v>
       </c>
-      <c r="H35" s="8">
+      <c r="H35" s="7">
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
       <c r="J35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L35" t="s">
-        <v>170</v>
-      </c>
-      <c r="M35" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M35" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2034,62 +2033,62 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>24</v>
+        <v>192</v>
       </c>
       <c r="F36" s="4">
-        <v>1</v>
-      </c>
-      <c r="G36" s="8">
+        <v>2</v>
+      </c>
+      <c r="G36" s="7">
         <v>4.37</v>
       </c>
-      <c r="H36" s="8">
-        <f t="shared" si="0"/>
-        <v>4.37</v>
+      <c r="H36" s="7">
+        <f t="shared" si="0"/>
+        <v>8.74</v>
       </c>
       <c r="J36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L36" t="s">
-        <v>170</v>
-      </c>
-      <c r="M36" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M36" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35"/>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B38" t="s">
         <v>9</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F38" s="4">
         <v>1</v>
       </c>
-      <c r="G38" s="8">
+      <c r="G38" s="7">
         <v>0.31</v>
       </c>
-      <c r="H38" s="8">
+      <c r="H38" s="7">
         <f t="shared" si="0"/>
         <v>0.31</v>
       </c>
       <c r="J38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L38" t="s">
-        <v>170</v>
-      </c>
-      <c r="M38" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M38" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2098,124 +2097,124 @@
         <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F39" s="4">
         <v>1</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="7">
         <v>0.24</v>
       </c>
-      <c r="H39" s="8">
+      <c r="H39" s="7">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
       <c r="J39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L39" t="s">
-        <v>170</v>
-      </c>
-      <c r="M39" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M39" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35"/>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F41" s="4">
         <v>2</v>
       </c>
       <c r="J41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L41" t="s">
-        <v>171</v>
-      </c>
-      <c r="M41" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M41" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" s="4">
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L42" t="s">
-        <v>171</v>
-      </c>
-      <c r="M42" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M42" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" s="4">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L43" t="s">
-        <v>171</v>
-      </c>
-      <c r="M43" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M43" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" t="s">
+        <v>142</v>
+      </c>
+      <c r="D44" t="s">
         <v>34</v>
       </c>
-      <c r="C44" t="s">
-        <v>143</v>
-      </c>
-      <c r="D44" t="s">
-        <v>35</v>
-      </c>
       <c r="F44" s="4">
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L44" t="s">
-        <v>171</v>
-      </c>
-      <c r="M44" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M44" s="6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2224,88 +2223,88 @@
         <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F45" s="4">
         <v>1</v>
       </c>
-      <c r="G45" s="8">
+      <c r="G45" s="7">
         <v>0.69</v>
       </c>
-      <c r="H45" s="8">
+      <c r="H45" s="7">
         <f>F45*G45</f>
         <v>0.69</v>
       </c>
       <c r="J45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L45" t="s">
-        <v>170</v>
-      </c>
-      <c r="M45" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M45" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F46" s="4">
         <v>2</v>
       </c>
-      <c r="G46" s="8">
+      <c r="G46" s="7">
         <v>4.6500000000000004</v>
       </c>
-      <c r="H46" s="8">
+      <c r="H46" s="7">
         <f>F46*G46</f>
         <v>9.3000000000000007</v>
       </c>
       <c r="J46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L46" t="s">
-        <v>170</v>
-      </c>
-      <c r="M46" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M46" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
+        <v>185</v>
+      </c>
+      <c r="C47" t="s">
         <v>186</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>187</v>
-      </c>
-      <c r="D47" t="s">
-        <v>188</v>
       </c>
       <c r="F47" s="4">
         <v>2</v>
       </c>
-      <c r="G47" s="8">
+      <c r="G47" s="7">
         <v>9.84</v>
       </c>
-      <c r="H47" s="8">
+      <c r="H47" s="7">
         <f>F47*G47</f>
         <v>19.68</v>
       </c>
       <c r="J47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L47" t="s">
-        <v>170</v>
-      </c>
-      <c r="M47" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M47" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2314,55 +2313,55 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F48" s="4">
         <v>3</v>
       </c>
       <c r="J48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L48" t="s">
-        <v>90</v>
-      </c>
-      <c r="M48" s="7" t="b">
+        <v>89</v>
+      </c>
+      <c r="M48" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
         <v>13</v>
       </c>
       <c r="C50" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F50" s="4">
         <v>1</v>
       </c>
-      <c r="G50" s="8">
+      <c r="G50" s="7">
         <v>3.34</v>
       </c>
-      <c r="H50" s="8">
+      <c r="H50" s="7">
         <f t="shared" si="0"/>
         <v>3.34</v>
       </c>
       <c r="J50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L50" t="s">
-        <v>170</v>
-      </c>
-      <c r="M50" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M50" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2372,62 +2371,62 @@
         <v>14</v>
       </c>
       <c r="C51" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F51" s="4">
         <v>1</v>
       </c>
-      <c r="G51" s="8">
+      <c r="G51" s="7">
         <v>14.81</v>
       </c>
-      <c r="H51" s="8">
+      <c r="H51" s="7">
         <f t="shared" si="0"/>
         <v>14.81</v>
       </c>
       <c r="J51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L51" t="s">
-        <v>168</v>
-      </c>
-      <c r="M51" s="7" t="b">
+        <v>167</v>
+      </c>
+      <c r="M51" s="6" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.35"/>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" t="s">
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D53" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F53" s="4">
         <v>1</v>
       </c>
-      <c r="G53" s="8">
+      <c r="G53" s="7">
         <v>0.38</v>
       </c>
-      <c r="H53" s="8">
+      <c r="H53" s="7">
         <f t="shared" si="0"/>
         <v>0.38</v>
       </c>
       <c r="J53" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L53" t="s">
-        <v>170</v>
-      </c>
-      <c r="M53" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M53" s="6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2436,152 +2435,152 @@
         <v>16</v>
       </c>
       <c r="C54" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F54" s="4">
         <v>1</v>
       </c>
-      <c r="G54" s="8">
+      <c r="G54" s="7">
         <v>0.39</v>
       </c>
-      <c r="H54" s="8">
+      <c r="H54" s="7">
         <f t="shared" si="0"/>
         <v>0.39</v>
       </c>
       <c r="J54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L54" t="s">
-        <v>170</v>
-      </c>
-      <c r="M54" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M54" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F55" s="4">
         <v>1</v>
       </c>
-      <c r="G55" s="8">
+      <c r="G55" s="7">
         <v>10.27</v>
       </c>
-      <c r="H55" s="8">
+      <c r="H55" s="7">
         <f t="shared" si="0"/>
         <v>10.27</v>
       </c>
       <c r="J55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L55" t="s">
-        <v>170</v>
-      </c>
-      <c r="M55" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M55" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" s="4">
+        <v>1</v>
+      </c>
+      <c r="G56" s="7">
+        <v>3.72</v>
+      </c>
+      <c r="H56" s="7">
+        <f t="shared" si="0"/>
+        <v>3.72</v>
+      </c>
+      <c r="J56" t="s">
+        <v>156</v>
+      </c>
+      <c r="L56" t="s">
+        <v>169</v>
+      </c>
+      <c r="M56" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N56" t="s">
         <v>111</v>
-      </c>
-      <c r="C56" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" s="4">
-        <v>1</v>
-      </c>
-      <c r="G56" s="8">
-        <v>3.72</v>
-      </c>
-      <c r="H56" s="8">
-        <f t="shared" si="0"/>
-        <v>3.72</v>
-      </c>
-      <c r="J56" t="s">
-        <v>157</v>
-      </c>
-      <c r="L56" t="s">
-        <v>170</v>
-      </c>
-      <c r="M56" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="N56" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" t="s">
         <v>179</v>
       </c>
-      <c r="C57" t="s">
+      <c r="E57" t="s">
         <v>180</v>
       </c>
-      <c r="E57" t="s">
-        <v>181</v>
-      </c>
       <c r="F57" s="4">
         <v>1</v>
       </c>
-      <c r="G57" s="8">
+      <c r="G57" s="7">
         <v>0.72</v>
       </c>
-      <c r="H57" s="8">
+      <c r="H57" s="7">
         <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
       <c r="J57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L57" t="s">
-        <v>170</v>
-      </c>
-      <c r="M57" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M57" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F58" s="4">
         <v>1</v>
       </c>
-      <c r="H58" s="8">
+      <c r="H58" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J58" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L58" t="s">
-        <v>171</v>
-      </c>
-      <c r="M58" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M58" s="6" t="b">
         <v>0</v>
       </c>
       <c r="N58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.35">
@@ -2589,85 +2588,85 @@
         <v>11</v>
       </c>
       <c r="C59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F59" s="4">
         <v>1</v>
       </c>
-      <c r="G59" s="8">
+      <c r="G59" s="7">
         <v>0.47</v>
       </c>
-      <c r="H59" s="8">
+      <c r="H59" s="7">
         <f t="shared" si="0"/>
         <v>0.47</v>
       </c>
       <c r="J59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L59" t="s">
-        <v>170</v>
-      </c>
-      <c r="M59" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M59" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" t="s">
+        <v>159</v>
+      </c>
+      <c r="D60" t="s">
         <v>140</v>
       </c>
-      <c r="C60" t="s">
-        <v>160</v>
-      </c>
-      <c r="D60" t="s">
-        <v>141</v>
-      </c>
       <c r="F60" s="4">
         <v>1</v>
       </c>
-      <c r="G60" s="8">
+      <c r="G60" s="7">
         <v>1.5</v>
       </c>
-      <c r="H60" s="8">
+      <c r="H60" s="7">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="J60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L60" t="s">
-        <v>170</v>
-      </c>
-      <c r="M60" s="7" t="b">
+        <v>169</v>
+      </c>
+      <c r="M60" s="6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.35"/>
     <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F62" s="4">
         <v>1</v>
       </c>
       <c r="J62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L62" t="s">
-        <v>171</v>
-      </c>
-      <c r="M62" s="7" t="b">
+        <v>170</v>
+      </c>
+      <c r="M62" s="6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>